<commit_message>
data: Add budget model to schema and sync Excel data files
- Added budget model (Model_ID=4) with 8 fields to Nexsus1_schema.xlsx
- Updated SAMPLE_payload_config.xlsx with budget field payload settings
- Added SAMPLE_budget_data.xlsx for budget sync testing
- Updated actual and master data files

This fixes Bug 5: Schema Excel file not pushed to git.
Railway was missing budget model definition, causing nexsus_search
validation to fail with "Model 'budget' not found in schema".

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/samples/Nexsus1_schema.xlsx
+++ b/samples/Nexsus1_schema.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KasunJ\MCP\Nexsus1\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5568E546-3E8F-43F8-B4F5-0C807B0CE875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46138DBD-BD7E-40B5-A2EC-F723DE52400D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11712" yWindow="12852" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="1" r:id="rId1"/>
     <sheet name="Instance_Config" sheetId="2" r:id="rId2"/>
     <sheet name="Model_Metadata" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="241">
   <si>
     <t>Field_ID</t>
   </si>
@@ -375,9 +388,6 @@
     <t>Positive=debit, negative=credit. SUM for totals. All values in AUD.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Config_Key</t>
   </si>
   <si>
@@ -705,9 +715,6 @@
     <t>Monthly Actuals</t>
   </si>
   <si>
-    <t>Monthly financial transactions by account and entity</t>
-  </si>
-  <si>
     <t>One row per account/month/entity combination</t>
   </si>
   <si>
@@ -723,9 +730,6 @@
     <t>Large dataset - use filters when possible. Month needs date conversion.</t>
   </si>
   <si>
-    <t>00000003-0002-0000-0000-000000000204</t>
-  </si>
-  <si>
     <t>Account_Name</t>
   </si>
   <si>
@@ -742,6 +746,18 @@
   </si>
   <si>
     <t>Qdrant_ID_for_FK</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>Monthly Budget numbers</t>
+  </si>
+  <si>
+    <t>Monthly budgeted financial transactions by account and entity</t>
+  </si>
+  <si>
+    <t>Monthly actual  financial transactions by account and entity</t>
   </si>
 </sst>
 </file>
@@ -777,8 +793,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,18 +1130,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,13 +1164,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" t="s">
         <v>236</v>
-      </c>
-      <c r="I1" t="s">
-        <v>237</v>
-      </c>
-      <c r="J1" t="s">
-        <v>239</v>
       </c>
       <c r="K1" t="s">
         <v>11</v>
@@ -1192,7 +1209,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -1242,7 +1259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102</v>
       </c>
@@ -1292,7 +1309,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>103</v>
       </c>
@@ -1342,7 +1359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -1392,7 +1409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>105</v>
       </c>
@@ -1442,7 +1459,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>106</v>
       </c>
@@ -1492,7 +1509,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>107</v>
       </c>
@@ -1542,7 +1559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>108</v>
       </c>
@@ -1550,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1592,7 +1609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>109</v>
       </c>
@@ -1600,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -1642,7 +1659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>110</v>
       </c>
@@ -1650,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -1692,7 +1709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>111</v>
       </c>
@@ -1700,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1742,7 +1759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>201</v>
       </c>
@@ -1783,7 +1800,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>202</v>
       </c>
@@ -1824,7 +1841,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>203</v>
       </c>
@@ -1865,7 +1882,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>204</v>
       </c>
@@ -1906,7 +1923,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>205</v>
       </c>
@@ -1947,7 +1964,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>206</v>
       </c>
@@ -1997,7 +2014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>207</v>
       </c>
@@ -2047,7 +2064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>208</v>
       </c>
@@ -2097,7 +2114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>209</v>
       </c>
@@ -2147,7 +2164,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>210</v>
       </c>
@@ -2197,7 +2214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>211</v>
       </c>
@@ -2247,7 +2264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>212</v>
       </c>
@@ -2288,7 +2305,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>213</v>
       </c>
@@ -2329,7 +2346,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>214</v>
       </c>
@@ -2379,7 +2396,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>215</v>
       </c>
@@ -2429,7 +2446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>216</v>
       </c>
@@ -2479,7 +2496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>217</v>
       </c>
@@ -2529,7 +2546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>218</v>
       </c>
@@ -2579,7 +2596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>219</v>
       </c>
@@ -2629,7 +2646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>220</v>
       </c>
@@ -2637,7 +2654,7 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D32" t="s">
         <v>74</v>
@@ -2679,7 +2696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>221</v>
       </c>
@@ -2729,7 +2746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>222</v>
       </c>
@@ -2779,7 +2796,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>223</v>
       </c>
@@ -2829,7 +2846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>224</v>
       </c>
@@ -2879,7 +2896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>225</v>
       </c>
@@ -2929,7 +2946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>226</v>
       </c>
@@ -2979,7 +2996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>227</v>
       </c>
@@ -3029,7 +3046,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>301</v>
       </c>
@@ -3079,7 +3096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>302</v>
       </c>
@@ -3087,7 +3104,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D41" t="s">
         <v>91</v>
@@ -3120,7 +3137,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>303</v>
       </c>
@@ -3170,7 +3187,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>304</v>
       </c>
@@ -3211,7 +3228,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>305</v>
       </c>
@@ -3225,7 +3242,7 @@
         <v>104</v>
       </c>
       <c r="E44" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="F44" t="s">
         <v>85</v>
@@ -3233,15 +3250,6 @@
       <c r="G44" t="s">
         <v>19</v>
       </c>
-      <c r="H44" t="s">
-        <v>25</v>
-      </c>
-      <c r="I44">
-        <v>2</v>
-      </c>
-      <c r="J44" t="s">
-        <v>233</v>
-      </c>
       <c r="K44" t="s">
         <v>105</v>
       </c>
@@ -3261,7 +3269,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>306</v>
       </c>
@@ -3302,7 +3310,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>307</v>
       </c>
@@ -3352,7 +3360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>308</v>
       </c>
@@ -3393,60 +3401,365 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48" t="s">
-        <v>20</v>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>401</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="E48" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="G48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H48" t="s">
-        <v>20</v>
-      </c>
-      <c r="I48" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="I48">
+        <v>2</v>
       </c>
       <c r="J48" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="K48" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="L48" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="M48" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="N48" t="s">
         <v>20</v>
       </c>
       <c r="O48" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="P48" t="s">
-        <v>20</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>402</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>231</v>
+      </c>
+      <c r="D49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" t="s">
+        <v>237</v>
+      </c>
+      <c r="G49" t="s">
+        <v>19</v>
+      </c>
+      <c r="K49" t="s">
+        <v>92</v>
+      </c>
+      <c r="L49" t="s">
+        <v>93</v>
+      </c>
+      <c r="M49" t="s">
+        <v>28</v>
+      </c>
+      <c r="N49" t="s">
+        <v>20</v>
+      </c>
+      <c r="O49" t="s">
+        <v>94</v>
+      </c>
+      <c r="P49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>403</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" t="s">
+        <v>97</v>
+      </c>
+      <c r="F50" t="s">
+        <v>237</v>
+      </c>
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>20</v>
+      </c>
+      <c r="I50" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" t="s">
+        <v>20</v>
+      </c>
+      <c r="K50" t="s">
+        <v>20</v>
+      </c>
+      <c r="L50" t="s">
+        <v>20</v>
+      </c>
+      <c r="M50" t="s">
+        <v>20</v>
+      </c>
+      <c r="N50" t="s">
+        <v>20</v>
+      </c>
+      <c r="O50" t="s">
+        <v>20</v>
+      </c>
+      <c r="P50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>404</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" t="s">
+        <v>237</v>
+      </c>
+      <c r="G51" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" t="s">
+        <v>98</v>
+      </c>
+      <c r="L51" t="s">
+        <v>99</v>
+      </c>
+      <c r="M51" t="s">
+        <v>100</v>
+      </c>
+      <c r="N51" t="s">
+        <v>101</v>
+      </c>
+      <c r="O51" t="s">
+        <v>102</v>
+      </c>
+      <c r="P51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>405</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" t="s">
+        <v>237</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" t="s">
+        <v>105</v>
+      </c>
+      <c r="L52" t="s">
+        <v>60</v>
+      </c>
+      <c r="M52" t="s">
+        <v>61</v>
+      </c>
+      <c r="N52" t="s">
+        <v>20</v>
+      </c>
+      <c r="O52" t="s">
+        <v>20</v>
+      </c>
+      <c r="P52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>406</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" t="s">
+        <v>237</v>
+      </c>
+      <c r="G53" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" t="s">
+        <v>107</v>
+      </c>
+      <c r="L53" t="s">
+        <v>108</v>
+      </c>
+      <c r="M53" t="s">
+        <v>109</v>
+      </c>
+      <c r="N53" t="s">
+        <v>20</v>
+      </c>
+      <c r="O53" t="s">
+        <v>20</v>
+      </c>
+      <c r="P53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>407</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" t="s">
+        <v>237</v>
+      </c>
+      <c r="G54" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" t="s">
+        <v>20</v>
+      </c>
+      <c r="I54" t="s">
+        <v>20</v>
+      </c>
+      <c r="J54" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" t="s">
+        <v>20</v>
+      </c>
+      <c r="L54" t="s">
+        <v>20</v>
+      </c>
+      <c r="M54" t="s">
+        <v>20</v>
+      </c>
+      <c r="N54" t="s">
+        <v>20</v>
+      </c>
+      <c r="O54" t="s">
+        <v>20</v>
+      </c>
+      <c r="P54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>408</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" t="s">
+        <v>53</v>
+      </c>
+      <c r="F55" t="s">
+        <v>237</v>
+      </c>
+      <c r="G55" t="s">
+        <v>19</v>
+      </c>
+      <c r="K55" t="s">
+        <v>112</v>
+      </c>
+      <c r="L55" t="s">
+        <v>113</v>
+      </c>
+      <c r="M55" t="s">
+        <v>114</v>
+      </c>
+      <c r="N55" t="s">
+        <v>20</v>
+      </c>
+      <c r="O55" t="s">
+        <v>115</v>
+      </c>
+      <c r="P55" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:I8 A46:I48 A45:B45 E45:I45 A44:D44 A43:D43 K43:V43 A42:I42 A41:B41 D41:I41 A33:I40 A32:B32 D32:I32 A13:I31 A9:B9 D9:I9 A10:B10 D10:I10 A11:B11 D11:I11 A12:B12 D12:I12 A1:G1 K1:V1 J2:V8 J46:V48 J45:V45 K44:V44 J42:V42 J41:V41 J33:V40 J32:V32 J13:V31 J9:V9 J10:V10 J11:V11 J12:V12 F43:G43 F44:G44" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:I8 A46:I47 A45:B45 E45:I45 A44:D44 A43:D43 K43:V43 A42:I42 A41:B41 D41:I41 A33:I40 A32:B32 D32:I32 A13:I31 A9:B9 D9:I9 A10:B10 D10:I10 A11:B11 D11:I11 A12:B12 D12:I12 A1:G1 K1:V1 J2:V8 J46:V47 J45:V45 K44:V44 J42:V42 J41:V41 J33:V40 J32:V32 J13:V31 J9:V9 J10:V10 J11:V11 J12:V12 F43:G43 F44:G44" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3456,451 +3769,451 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
         <v>118</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>119</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>120</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>121</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>122</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>123</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>125</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>127</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>128</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>129</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>130</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>132</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" t="s">
         <v>133</v>
       </c>
-      <c r="C3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" t="s">
         <v>134</v>
       </c>
-      <c r="E3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>135</v>
       </c>
-      <c r="G3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>136</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" t="s">
         <v>137</v>
       </c>
-      <c r="C4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
         <v>138</v>
       </c>
-      <c r="E4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>139</v>
       </c>
-      <c r="G4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>140</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
         <v>141</v>
       </c>
-      <c r="C5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" t="s">
         <v>142</v>
       </c>
-      <c r="E5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>143</v>
       </c>
-      <c r="G5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>144</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" t="s">
         <v>145</v>
       </c>
-      <c r="C6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" t="s">
         <v>146</v>
       </c>
-      <c r="E6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>147</v>
       </c>
-      <c r="G6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>148</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>149</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>150</v>
-      </c>
-      <c r="D7" t="s">
-        <v>151</v>
       </c>
       <c r="E7" t="s">
         <v>85</v>
       </c>
       <c r="F7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>152</v>
       </c>
-      <c r="G7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" t="s">
         <v>154</v>
-      </c>
-      <c r="C8" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" t="s">
-        <v>155</v>
       </c>
       <c r="E8" t="s">
         <v>85</v>
       </c>
       <c r="F8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>156</v>
       </c>
-      <c r="G8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>157</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" t="s">
         <v>158</v>
       </c>
-      <c r="C9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" t="s">
         <v>159</v>
       </c>
-      <c r="E9" t="s">
-        <v>129</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>160</v>
       </c>
-      <c r="G9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>161</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="s">
         <v>162</v>
-      </c>
-      <c r="C10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" t="s">
-        <v>163</v>
       </c>
       <c r="E10" t="s">
         <v>85</v>
       </c>
       <c r="F10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>164</v>
       </c>
-      <c r="G10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>165</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>166</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>167</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" t="s">
         <v>168</v>
       </c>
-      <c r="E11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>169</v>
       </c>
-      <c r="G11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>170</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" t="s">
         <v>171</v>
       </c>
-      <c r="C12" t="s">
-        <v>167</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>172</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>173</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>174</v>
       </c>
-      <c r="G12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>175</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" t="s">
         <v>176</v>
       </c>
-      <c r="C13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>172</v>
+      </c>
+      <c r="F13" t="s">
         <v>177</v>
       </c>
-      <c r="E13" t="s">
-        <v>173</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>178</v>
       </c>
-      <c r="G13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>179</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D14" t="s">
         <v>180</v>
       </c>
-      <c r="C14" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" t="s">
         <v>181</v>
       </c>
-      <c r="E14" t="s">
-        <v>129</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>182</v>
       </c>
-      <c r="G14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>183</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" t="s">
         <v>184</v>
       </c>
-      <c r="C15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>185</v>
       </c>
-      <c r="E15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F15" t="s">
-        <v>182</v>
-      </c>
-      <c r="G15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>186</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>187</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>188</v>
-      </c>
-      <c r="D16" t="s">
-        <v>189</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" t="s">
+        <v>189</v>
+      </c>
+      <c r="G16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>190</v>
       </c>
-      <c r="G16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>191</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" t="s">
         <v>192</v>
-      </c>
-      <c r="C17" t="s">
-        <v>188</v>
-      </c>
-      <c r="D17" t="s">
-        <v>193</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
       </c>
       <c r="F17" t="s">
+        <v>193</v>
+      </c>
+      <c r="G17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>194</v>
       </c>
-      <c r="G17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>195</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D18" t="s">
         <v>196</v>
       </c>
-      <c r="C18" t="s">
-        <v>188</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" t="s">
         <v>197</v>
       </c>
-      <c r="E18" t="s">
-        <v>166</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>198</v>
       </c>
-      <c r="G18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>199</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" t="s">
         <v>200</v>
       </c>
-      <c r="C19" t="s">
-        <v>188</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" t="s">
         <v>201</v>
       </c>
-      <c r="E19" t="s">
-        <v>173</v>
-      </c>
-      <c r="F19" t="s">
-        <v>202</v>
-      </c>
       <c r="G19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3913,15 +4226,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3929,37 +4242,37 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" t="s">
         <v>203</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>204</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>205</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>206</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>207</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>208</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>209</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>210</v>
       </c>
-      <c r="K1" t="s">
-        <v>211</v>
-      </c>
       <c r="L1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3967,13 +4280,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" t="s">
         <v>212</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>213</v>
-      </c>
-      <c r="E2" t="s">
-        <v>214</v>
       </c>
       <c r="F2">
         <v>48</v>
@@ -3982,22 +4295,22 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2" t="s">
         <v>215</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>216</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>217</v>
       </c>
-      <c r="K2" t="s">
-        <v>218</v>
-      </c>
       <c r="L2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4005,13 +4318,13 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" t="s">
         <v>219</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>220</v>
-      </c>
-      <c r="E3" t="s">
-        <v>221</v>
       </c>
       <c r="F3">
         <v>560</v>
@@ -4020,22 +4333,22 @@
         <v>19</v>
       </c>
       <c r="H3" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" t="s">
         <v>222</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>223</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>224</v>
       </c>
-      <c r="K3" t="s">
-        <v>225</v>
-      </c>
       <c r="L3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4043,13 +4356,13 @@
         <v>85</v>
       </c>
       <c r="C4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" t="s">
         <v>226</v>
-      </c>
-      <c r="D4" t="s">
-        <v>227</v>
-      </c>
-      <c r="E4" t="s">
-        <v>228</v>
       </c>
       <c r="F4">
         <v>15000</v>
@@ -4058,25 +4371,63 @@
         <v>19</v>
       </c>
       <c r="H4" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" t="s">
+        <v>228</v>
+      </c>
+      <c r="J4" t="s">
         <v>229</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>230</v>
       </c>
-      <c r="J4" t="s">
-        <v>231</v>
-      </c>
-      <c r="K4" t="s">
-        <v>232</v>
-      </c>
       <c r="L4" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F5">
+        <v>15000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>227</v>
+      </c>
+      <c r="I5" t="s">
+        <v>228</v>
+      </c>
+      <c r="J5" t="s">
+        <v>229</v>
+      </c>
+      <c r="K5" t="s">
+        <v>230</v>
+      </c>
+      <c r="L5" s="1">
+        <v>45666</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:L1 A3:L4 A2:F2 H2:L2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:L1 A3:L3 A2:F2 H2:L2 A4:C4 E4:L4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>